<commit_message>
age-stratification and hospitals are now working
</commit_message>
<xml_diff>
--- a/data/interim/model_parameters/COVID19_SEIRD/hospitals/0_10_20_30_40_50_60_70_80/sciensano_hospital_parameters.xlsx
+++ b/data/interim/model_parameters/COVID19_SEIRD/hospitals/0_10_20_30_40_50_60_70_80/sciensano_hospital_parameters.xlsx
@@ -721,10 +721,10 @@
         <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>0.98</v>
+        <v>0.981</v>
       </c>
       <c r="I4" t="n">
-        <v>0.98</v>
+        <v>0.981</v>
       </c>
       <c r="J4" t="n">
         <v>0.977</v>
@@ -733,7 +733,7 @@
         <v>0.983</v>
       </c>
       <c r="L4" t="n">
-        <v>0.971</v>
+        <v>0.9710000000000001</v>
       </c>
       <c r="M4" t="n">
         <v>0.988</v>
@@ -824,13 +824,13 @@
         <v>0.87</v>
       </c>
       <c r="J5" t="n">
-        <v>0.863</v>
+        <v>0.862</v>
       </c>
       <c r="K5" t="n">
-        <v>0.877</v>
+        <v>0.878</v>
       </c>
       <c r="L5" t="n">
-        <v>0.8489749999999999</v>
+        <v>0.847</v>
       </c>
       <c r="M5" t="n">
         <v>0.89</v>
@@ -842,13 +842,13 @@
         <v>0.012</v>
       </c>
       <c r="P5" t="n">
-        <v>0.01</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="Q5" t="n">
         <v>0.014</v>
       </c>
       <c r="R5" t="n">
-        <v>0.006</v>
+        <v>0.005475000000000002</v>
       </c>
       <c r="S5" t="n">
         <v>0.019</v>
@@ -872,22 +872,22 @@
         <v>0</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.08935830429732869</v>
+        <v>0.09163486005089058</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.08935830429732869</v>
+        <v>0.09163486005089058</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.072992700729927</v>
+        <v>0.07349568267674042</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.1073964168839092</v>
+        <v>0.1094890510948905</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.04385804840568574</v>
+        <v>0.04540437383948834</v>
       </c>
       <c r="AE5" t="n">
-        <v>0.1415115211220571</v>
+        <v>0.1462462462462462</v>
       </c>
     </row>
     <row r="6">
@@ -915,76 +915,76 @@
         <v>0.007619047619047619</v>
       </c>
       <c r="H6" t="n">
-        <v>0.9106425702811245</v>
+        <v>0.9098196392785571</v>
       </c>
       <c r="I6" t="n">
-        <v>0.9106425702811245</v>
+        <v>0.9098196392785571</v>
       </c>
       <c r="J6" t="n">
-        <v>0.904</v>
+        <v>0.9038076152304609</v>
       </c>
       <c r="K6" t="n">
-        <v>0.9159159159159159</v>
+        <v>0.9159369369369369</v>
       </c>
       <c r="L6" t="n">
-        <v>0.8909972722722723</v>
+        <v>0.8938380765535074</v>
       </c>
       <c r="M6" t="n">
-        <v>0.926855537902632</v>
+        <v>0.9269269269269269</v>
       </c>
       <c r="N6" t="n">
-        <v>0.01504513540621866</v>
+        <v>0.01601601601601602</v>
       </c>
       <c r="O6" t="n">
-        <v>0.01504513540621866</v>
+        <v>0.01601601601601602</v>
       </c>
       <c r="P6" t="n">
-        <v>0.01300975975975976</v>
+        <v>0.01302605210420842</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.01803607214428858</v>
+        <v>0.01806323493092343</v>
       </c>
       <c r="R6" t="n">
         <v>0.008016032064128256</v>
       </c>
       <c r="S6" t="n">
-        <v>0.02402402402402402</v>
+        <v>0.02501313813813814</v>
       </c>
       <c r="T6" t="n">
-        <v>0.007650273224043716</v>
+        <v>0.007667031763417305</v>
       </c>
       <c r="U6" t="n">
-        <v>0.007650273224043716</v>
+        <v>0.007667031763417305</v>
       </c>
       <c r="V6" t="n">
-        <v>0.005500550055005501</v>
+        <v>0.005488474204171241</v>
       </c>
       <c r="W6" t="n">
-        <v>0.009711359013609007</v>
+        <v>0.009849523416922116</v>
       </c>
       <c r="X6" t="n">
-        <v>0.002212389380530973</v>
+        <v>0.002709165751258436</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.01411509229098806</v>
+        <v>0.01416200815689141</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.09523809523809523</v>
+        <v>0.09375</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.09523809523809523</v>
+        <v>0.09375</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.075</v>
+        <v>0.07486702127659574</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.1170212765957447</v>
+        <v>0.1168831168831169</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.0375</v>
+        <v>0.04040404040404041</v>
       </c>
       <c r="AE6" t="n">
-        <v>0.160928809788654</v>
+        <v>0.1547435897435897</v>
       </c>
     </row>
     <row r="7">
@@ -1012,76 +1012,76 @@
         <v>0.01177730192719486</v>
       </c>
       <c r="H7" t="n">
-        <v>0.8978978978978979</v>
+        <v>0.897</v>
       </c>
       <c r="I7" t="n">
-        <v>0.8978978978978979</v>
+        <v>0.897</v>
       </c>
       <c r="J7" t="n">
-        <v>0.8908908908908909</v>
+        <v>0.89</v>
       </c>
       <c r="K7" t="n">
-        <v>0.9039039039039038</v>
+        <v>0.9029029029029029</v>
       </c>
       <c r="L7" t="n">
-        <v>0.8788788788788788</v>
+        <v>0.877</v>
       </c>
       <c r="M7" t="n">
-        <v>0.916</v>
+        <v>0.913913913913914</v>
       </c>
       <c r="N7" t="n">
-        <v>0.027</v>
+        <v>0.02655220883534137</v>
       </c>
       <c r="O7" t="n">
-        <v>0.027</v>
+        <v>0.02655220883534137</v>
       </c>
       <c r="P7" t="n">
-        <v>0.024</v>
+        <v>0.02302302302302302</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.03003003003003003</v>
+        <v>0.03006765788347005</v>
       </c>
       <c r="R7" t="n">
-        <v>0.018</v>
+        <v>0.01702511629866339</v>
       </c>
       <c r="S7" t="n">
-        <v>0.0370750779392285</v>
+        <v>0.03707414829659319</v>
       </c>
       <c r="T7" t="n">
-        <v>0.01126126126126126</v>
+        <v>0.01128031943726921</v>
       </c>
       <c r="U7" t="n">
-        <v>0.01126126126126126</v>
+        <v>0.01128031943726921</v>
       </c>
       <c r="V7" t="n">
-        <v>0.008976159200374447</v>
+        <v>0.008946046267481534</v>
       </c>
       <c r="W7" t="n">
-        <v>0.0136518771331058</v>
+        <v>0.01434878587196468</v>
       </c>
       <c r="X7" t="n">
-        <v>0.005418704084430676</v>
+        <v>0.005521660385642677</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.01971630659951451</v>
+        <v>0.01882720061613327</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.1578947368421053</v>
+        <v>0.160188679245283</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.1578947368421053</v>
+        <v>0.160188679245283</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.1333333333333333</v>
+        <v>0.134020618556701</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.183066681584247</v>
+        <v>0.1834862385321101</v>
       </c>
       <c r="AD7" t="n">
-        <v>0.09344707672245164</v>
+        <v>0.08919289250353607</v>
       </c>
       <c r="AE7" t="n">
-        <v>0.2336448598130841</v>
+        <v>0.2319555868000991</v>
       </c>
     </row>
     <row r="8">
@@ -1109,76 +1109,76 @@
         <v>0.02119700748129676</v>
       </c>
       <c r="H8" t="n">
-        <v>0.8578578578578578</v>
+        <v>0.8582168674698796</v>
       </c>
       <c r="I8" t="n">
-        <v>0.8578578578578578</v>
+        <v>0.8582168674698796</v>
       </c>
       <c r="J8" t="n">
-        <v>0.8508508508508509</v>
+        <v>0.85</v>
       </c>
       <c r="K8" t="n">
-        <v>0.8648648648648649</v>
+        <v>0.8656304585097979</v>
       </c>
       <c r="L8" t="n">
-        <v>0.8368368368368369</v>
+        <v>0.8358358358358359</v>
       </c>
       <c r="M8" t="n">
-        <v>0.8786389479058416</v>
+        <v>0.879765422393306</v>
       </c>
       <c r="N8" t="n">
-        <v>0.04108216432865731</v>
+        <v>0.04104104104104104</v>
       </c>
       <c r="O8" t="n">
-        <v>0.04108216432865731</v>
+        <v>0.04104104104104104</v>
       </c>
       <c r="P8" t="n">
-        <v>0.03703703703703703</v>
+        <v>0.03702777777777778</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.04509018036072145</v>
+        <v>0.04604604604604605</v>
       </c>
       <c r="R8" t="n">
-        <v>0.02908726178535607</v>
+        <v>0.02905811623246493</v>
       </c>
       <c r="S8" t="n">
-        <v>0.05321285140562249</v>
+        <v>0.05413953109736242</v>
       </c>
       <c r="T8" t="n">
-        <v>0.02099126078122578</v>
+        <v>0.02121397319258282</v>
       </c>
       <c r="U8" t="n">
-        <v>0.02099126078122578</v>
+        <v>0.02121397319258282</v>
       </c>
       <c r="V8" t="n">
         <v>0.01785183455070494</v>
       </c>
       <c r="W8" t="n">
-        <v>0.02459016393442623</v>
+        <v>0.02448819296645384</v>
       </c>
       <c r="X8" t="n">
-        <v>0.01270171225669999</v>
+        <v>0.01282051282051282</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.03183962264150943</v>
+        <v>0.03119939320354708</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.1605839416058394</v>
+        <v>0.1620669965740388</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.1605839416058394</v>
+        <v>0.1620669965740388</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.1397058823529412</v>
+        <v>0.1397788258253375</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.1818181818181818</v>
+        <v>0.1824447622805287</v>
       </c>
       <c r="AD8" t="n">
-        <v>0.1014492753623188</v>
+        <v>0.1017496054448609</v>
       </c>
       <c r="AE8" t="n">
-        <v>0.2272894385026737</v>
+        <v>0.2222069269313363</v>
       </c>
     </row>
     <row r="9">
@@ -1206,76 +1206,76 @@
         <v>0.03681214421252372</v>
       </c>
       <c r="H9" t="n">
-        <v>0.8092369477911646</v>
+        <v>0.8086172344689379</v>
       </c>
       <c r="I9" t="n">
-        <v>0.8092369477911646</v>
+        <v>0.8086172344689379</v>
       </c>
       <c r="J9" t="n">
-        <v>0.8008008008008008</v>
+        <v>0.8006042296072508</v>
       </c>
       <c r="K9" t="n">
         <v>0.8174523570712137</v>
       </c>
       <c r="L9" t="n">
-        <v>0.7843530591775326</v>
+        <v>0.7845691382765531</v>
       </c>
       <c r="M9" t="n">
-        <v>0.8324974924774323</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="N9" t="n">
-        <v>0.08032128514056225</v>
+        <v>0.0802407221664995</v>
       </c>
       <c r="O9" t="n">
-        <v>0.08032128514056225</v>
+        <v>0.0802407221664995</v>
       </c>
       <c r="P9" t="n">
         <v>0.07429718875502007</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.08634538152610442</v>
+        <v>0.08610765073690926</v>
       </c>
       <c r="R9" t="n">
-        <v>0.06431999354200722</v>
+        <v>0.06516129048468049</v>
       </c>
       <c r="S9" t="n">
-        <v>0.09829488465396188</v>
+        <v>0.09628886659979939</v>
       </c>
       <c r="T9" t="n">
-        <v>0.03663003663003663</v>
+        <v>0.03625971502590673</v>
       </c>
       <c r="U9" t="n">
-        <v>0.03663003663003663</v>
+        <v>0.03625971502590673</v>
       </c>
       <c r="V9" t="n">
-        <v>0.03213844252163164</v>
+        <v>0.0322180916976456</v>
       </c>
       <c r="W9" t="n">
-        <v>0.04121212121212121</v>
+        <v>0.04054482238892886</v>
       </c>
       <c r="X9" t="n">
-        <v>0.02417226010456172</v>
+        <v>0.02454971410419314</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.0506367379425405</v>
+        <v>0.04915415951972556</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.2639593908629442</v>
+        <v>0.2661571000214179</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.2639593908629442</v>
+        <v>0.2661571000214179</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.2419354838709677</v>
+        <v>0.245048019207683</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.2857142857142857</v>
+        <v>0.2848993498374593</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.2</v>
+        <v>0.2025279123657047</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.3264248704663212</v>
+        <v>0.3299763635439435</v>
       </c>
     </row>
     <row r="10">
@@ -1303,22 +1303,22 @@
         <v>0.07581830327321309</v>
       </c>
       <c r="H10" t="n">
-        <v>0.7590361445783133</v>
+        <v>0.7598798798798798</v>
       </c>
       <c r="I10" t="n">
-        <v>0.7590361445783133</v>
+        <v>0.7598798798798798</v>
       </c>
       <c r="J10" t="n">
-        <v>0.7497497497497497</v>
+        <v>0.7492477432296891</v>
       </c>
       <c r="K10" t="n">
-        <v>0.7680722891566265</v>
+        <v>0.7685370741482966</v>
       </c>
       <c r="L10" t="n">
-        <v>0.7324582213574592</v>
+        <v>0.7298199554976663</v>
       </c>
       <c r="M10" t="n">
-        <v>0.7859314070351759</v>
+        <v>0.7847557678170411</v>
       </c>
       <c r="N10" t="n">
         <v>0.1643286573146293</v>
@@ -1327,52 +1327,52 @@
         <v>0.1643286573146293</v>
       </c>
       <c r="P10" t="n">
-        <v>0.156312625250501</v>
+        <v>0.1571571571571572</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.1721721721721722</v>
+        <v>0.172043043043043</v>
       </c>
       <c r="R10" t="n">
-        <v>0.1411411411411412</v>
+        <v>0.1412083175359728</v>
       </c>
       <c r="S10" t="n">
-        <v>0.1877557213779742</v>
+        <v>0.1867020541082164</v>
       </c>
       <c r="T10" t="n">
-        <v>0.07567567567567568</v>
+        <v>0.07572739345647712</v>
       </c>
       <c r="U10" t="n">
-        <v>0.07567567567567568</v>
+        <v>0.07572739345647712</v>
       </c>
       <c r="V10" t="n">
-        <v>0.06933333333333333</v>
+        <v>0.06948921398462683</v>
       </c>
       <c r="W10" t="n">
-        <v>0.08238416988416988</v>
+        <v>0.08226437000313597</v>
       </c>
       <c r="X10" t="n">
-        <v>0.05812417437252312</v>
+        <v>0.05760185723827375</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.09480805958747134</v>
+        <v>0.09440262699665479</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.4430379746835443</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.4430379746835443</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="AB10" t="n">
-        <v>0.4214796871536683</v>
+        <v>0.424308439329039</v>
       </c>
       <c r="AC10" t="n">
-        <v>0.46484375</v>
+        <v>0.4643647281921618</v>
       </c>
       <c r="AD10" t="n">
-        <v>0.3811475409836065</v>
+        <v>0.3823839662447257</v>
       </c>
       <c r="AE10" t="n">
-        <v>0.5083350840336134</v>
+        <v>0.5021948051948052</v>
       </c>
     </row>
     <row r="11">
@@ -1400,73 +1400,73 @@
         <v>0.1720401691331924</v>
       </c>
       <c r="H11" t="n">
-        <v>0.7827827827827828</v>
+        <v>0.7838516908868667</v>
       </c>
       <c r="I11" t="n">
-        <v>0.7827827827827828</v>
+        <v>0.7838516908868667</v>
       </c>
       <c r="J11" t="n">
-        <v>0.7743229689067201</v>
+        <v>0.7755511022044088</v>
       </c>
       <c r="K11" t="n">
-        <v>0.7919597989949749</v>
+        <v>0.7927927927927928</v>
       </c>
       <c r="L11" t="n">
-        <v>0.7567567567567568</v>
+        <v>0.76024749498998</v>
       </c>
       <c r="M11" t="n">
-        <v>0.8084252758274825</v>
+        <v>0.807431730931743</v>
       </c>
       <c r="N11" t="n">
-        <v>0.2660321285140562</v>
+        <v>0.2665330661322645</v>
       </c>
       <c r="O11" t="n">
-        <v>0.2660321285140562</v>
+        <v>0.2665330661322645</v>
       </c>
       <c r="P11" t="n">
-        <v>0.2570210843373494</v>
+        <v>0.2575150300601202</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.2755511022044088</v>
+        <v>0.2750688188188188</v>
       </c>
       <c r="R11" t="n">
-        <v>0.2394789579158317</v>
+        <v>0.2408420945996096</v>
       </c>
       <c r="S11" t="n">
-        <v>0.2945936641895461</v>
+        <v>0.2934475808473804</v>
       </c>
       <c r="T11" t="n">
-        <v>0.17207800422</v>
+        <v>0.1719543913614146</v>
       </c>
       <c r="U11" t="n">
-        <v>0.17207800422</v>
+        <v>0.1719543913614146</v>
       </c>
       <c r="V11" t="n">
-        <v>0.1625487646293888</v>
+        <v>0.1625761553520804</v>
       </c>
       <c r="W11" t="n">
-        <v>0.1819616036245265</v>
+        <v>0.1825119493289804</v>
       </c>
       <c r="X11" t="n">
-        <v>0.1457741947905669</v>
+        <v>0.1465863425831045</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.1994950287061328</v>
+        <v>0.1979448718463763</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.6036451197741521</v>
+        <v>0.6026785714285714</v>
       </c>
       <c r="AA11" t="n">
-        <v>0.6036451197741521</v>
+        <v>0.6026785714285714</v>
       </c>
       <c r="AB11" t="n">
-        <v>0.5813167818981773</v>
+        <v>0.5802678571428572</v>
       </c>
       <c r="AC11" t="n">
-        <v>0.6255761864571836</v>
+        <v>0.6286067892503536</v>
       </c>
       <c r="AD11" t="n">
-        <v>0.5360189735189734</v>
+        <v>0.5309557383470427</v>
       </c>
       <c r="AE11" t="n">
         <v>0.6666666666666666</v>
@@ -1506,67 +1506,67 @@
         <v>0.9115355449278586</v>
       </c>
       <c r="K12" t="n">
-        <v>0.923</v>
+        <v>0.9237713139418254</v>
       </c>
       <c r="L12" t="n">
-        <v>0.8994949597079968</v>
+        <v>0.8989272042854196</v>
       </c>
       <c r="M12" t="n">
-        <v>0.933933933933934</v>
+        <v>0.9327663462274374</v>
       </c>
       <c r="N12" t="n">
-        <v>0.4044044044044044</v>
+        <v>0.4046184738955823</v>
       </c>
       <c r="O12" t="n">
-        <v>0.4044044044044044</v>
+        <v>0.4046184738955823</v>
       </c>
       <c r="P12" t="n">
-        <v>0.3937875751503006</v>
+        <v>0.3945323335383576</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.4154154154154154</v>
+        <v>0.41528815676258</v>
       </c>
       <c r="R12" t="n">
-        <v>0.3743680741925476</v>
+        <v>0.3769393216080402</v>
       </c>
       <c r="S12" t="n">
-        <v>0.4357429718875502</v>
+        <v>0.4348697394789579</v>
       </c>
       <c r="T12" t="n">
-        <v>0.3737650694959062</v>
+        <v>0.3735667155862595</v>
       </c>
       <c r="U12" t="n">
-        <v>0.3737650694959062</v>
+        <v>0.3735667155862595</v>
       </c>
       <c r="V12" t="n">
-        <v>0.3628415300546448</v>
+        <v>0.3622988906693843</v>
       </c>
       <c r="W12" t="n">
-        <v>0.3844444444444444</v>
+        <v>0.3837341285109658</v>
       </c>
       <c r="X12" t="n">
-        <v>0.3409010535166683</v>
+        <v>0.3418275723630577</v>
       </c>
       <c r="Y12" t="n">
-        <v>0.4051856473079249</v>
+        <v>0.4037115318674725</v>
       </c>
       <c r="Z12" t="n">
-        <v>0.7529411764705882</v>
+        <v>0.7528089887640449</v>
       </c>
       <c r="AA12" t="n">
-        <v>0.7529411764705882</v>
+        <v>0.7528089887640449</v>
       </c>
       <c r="AB12" t="n">
-        <v>0.7208447332421341</v>
+        <v>0.72</v>
       </c>
       <c r="AC12" t="n">
-        <v>0.7837837837837838</v>
+        <v>0.7857142857142857</v>
       </c>
       <c r="AD12" t="n">
-        <v>0.6533194444444445</v>
+        <v>0.6535769230769231</v>
       </c>
       <c r="AE12" t="n">
-        <v>0.8431431608788093</v>
+        <v>0.8395061728395061</v>
       </c>
     </row>
     <row r="13">
@@ -1594,76 +1594,76 @@
         <v>0.1661084701815039</v>
       </c>
       <c r="H13" t="n">
-        <v>0.8378650553877141</v>
+        <v>0.8371746987951807</v>
       </c>
       <c r="I13" t="n">
-        <v>0.8378650553877141</v>
+        <v>0.8371746987951807</v>
       </c>
       <c r="J13" t="n">
-        <v>0.83</v>
+        <v>0.8286573146292585</v>
       </c>
       <c r="K13" t="n">
-        <v>0.846</v>
+        <v>0.8454202970356853</v>
       </c>
       <c r="L13" t="n">
-        <v>0.8142570281124498</v>
+        <v>0.8155341776833507</v>
       </c>
       <c r="M13" t="n">
-        <v>0.8600040241448691</v>
+        <v>0.8622557612778274</v>
       </c>
       <c r="N13" t="n">
-        <v>0.2146439317953862</v>
+        <v>0.2151452960498187</v>
       </c>
       <c r="O13" t="n">
-        <v>0.2146439317953862</v>
+        <v>0.2151452960498187</v>
       </c>
       <c r="P13" t="n">
         <v>0.2062062062062062</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.2232232232232232</v>
+        <v>0.2238955823293173</v>
       </c>
       <c r="R13" t="n">
-        <v>0.1885656970912738</v>
+        <v>0.1897735707121364</v>
       </c>
       <c r="S13" t="n">
-        <v>0.2394789579158317</v>
+        <v>0.2396994861725155</v>
       </c>
       <c r="T13" t="n">
-        <v>0.166058386058386</v>
+        <v>0.1650543923265879</v>
       </c>
       <c r="U13" t="n">
-        <v>0.166058386058386</v>
+        <v>0.1650543923265879</v>
       </c>
       <c r="V13" t="n">
-        <v>0.1573301549463647</v>
+        <v>0.1567004861551469</v>
       </c>
       <c r="W13" t="n">
-        <v>0.1744926636165421</v>
+        <v>0.1732894258490518</v>
       </c>
       <c r="X13" t="n">
-        <v>0.1409952606635071</v>
+        <v>0.1389973263165031</v>
       </c>
       <c r="Y13" t="n">
-        <v>0.1899053539426523</v>
+        <v>0.1899597576084187</v>
       </c>
       <c r="Z13" t="n">
-        <v>0.4630872483221476</v>
+        <v>0.4632509412342446</v>
       </c>
       <c r="AA13" t="n">
-        <v>0.4630872483221476</v>
+        <v>0.4632509412342446</v>
       </c>
       <c r="AB13" t="n">
-        <v>0.4375</v>
+        <v>0.440188679245283</v>
       </c>
       <c r="AC13" t="n">
-        <v>0.4902277039848197</v>
+        <v>0.4924028822055138</v>
       </c>
       <c r="AD13" t="n">
-        <v>0.3870919738863287</v>
+        <v>0.3944725028058361</v>
       </c>
       <c r="AE13" t="n">
-        <v>0.5384615384615384</v>
+        <v>0.5548832271762207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>